<commit_message>
Tested all other API calls of the Library API using excel Utilities and generated log files
</commit_message>
<xml_diff>
--- a/testData/addBookData.xlsx
+++ b/testData/addBookData.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://planittesting-my.sharepoint.com/personal/ryadav_planittesting_com/Documents/Desktop/Cucumber_BDD_API_Framework/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61763CF5-410D-4581-B327-342D85C163F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{61763CF5-410D-4581-B327-342D85C163F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A35ADC5C-8441-40F8-9918-00450FA5E614}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Add Book" sheetId="1" r:id="rId1"/>
+    <sheet name="Book Details" sheetId="1" r:id="rId1"/>
+    <sheet name="Delete Book" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -77,6 +78,24 @@
   </si>
   <si>
     <t>mno</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>abc1245</t>
+  </si>
+  <si>
+    <t>def2378</t>
+  </si>
+  <si>
+    <t>ghi4521</t>
+  </si>
+  <si>
+    <t>jkl3690</t>
+  </si>
+  <si>
+    <t>mno5987</t>
   </si>
 </sst>
 </file>
@@ -141,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -149,6 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,6 +184,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -554,4 +578,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AA3A626-6EA4-4670-A567-66E4E8E954AD}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>